<commit_message>
limpando o código e add funcoes
</commit_message>
<xml_diff>
--- a/testes_antes_da_main/teste.xlsx
+++ b/testes_antes_da_main/teste.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -552,6 +552,295 @@
         </is>
       </c>
       <c r="C8" t="inlineStr">
+        <is>
+          <t>3,949,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>3,949,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>3,949,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>3,949,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>3.949.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
         <is>
           <t>3,949,90</t>
         </is>

</xml_diff>

<commit_message>
criei um layout e mais funções
</commit_message>
<xml_diff>
--- a/testes_antes_da_main/teste.xlsx
+++ b/testes_antes_da_main/teste.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -841,6 +841,57 @@
         </is>
       </c>
       <c r="C25" t="inlineStr">
+        <is>
+          <t>3,949,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>3,949,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>3,949,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
         <is>
           <t>3,949,90</t>
         </is>

</xml_diff>

<commit_message>
pesquisa por lm no melgorando o codigo
</commit_message>
<xml_diff>
--- a/testes_antes_da_main/teste.xlsx
+++ b/testes_antes_da_main/teste.xlsx
@@ -3,11 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Plan1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Planilha1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,6 +30,14 @@
       <family val="2"/>
       <b val="1"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,11 +60,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,10 +431,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -452,17 +461,19 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>55555</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>casa</t>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>99.99</t>
+          <t>3,999,00</t>
         </is>
       </c>
     </row>
@@ -479,14 +490,25 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3,949,90</t>
+          <t>3,999,00</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="C4">
-        <f>TYPE(C3)</f>
-        <v/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3,999.00</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -502,7 +524,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3,949,90</t>
+          <t>3,999,00</t>
         </is>
       </c>
     </row>
@@ -519,7 +541,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3,949,90</t>
+          <t>3.999.00</t>
         </is>
       </c>
     </row>
@@ -536,7 +558,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3,949,90</t>
+          <t>3,999.00</t>
         </is>
       </c>
     </row>
@@ -553,7 +575,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>3,949,90</t>
+          <t>3,999,00</t>
         </is>
       </c>
     </row>
@@ -570,36 +592,36 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>,90</t>
+          <t>3,999,00</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>91697550</t>
+          <t>90991026</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+          <t>Ar Condicionado Split Frio 18000 BTUs 220V Elite Series A1 TCL</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>,90</t>
+          <t>2,999,00</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>91697550</t>
+          <t>87321941</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+          <t>Lixeira para Cozinha 12L Metal Inox Pedal Prata Brinox</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -611,29 +633,29 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>91697550</t>
+          <t>89031495</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+          <t>Ar Condicionado Split Inverter 9000BTUs Frio 220V TCL</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>,90</t>
+          <t>1,779,90</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>91697550</t>
+          <t>87321941</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+          <t>Lixeira para Cozinha 12L Metal Inox Pedal Prata Brinox</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -645,12 +667,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>91697550</t>
+          <t>87321941</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+          <t>Lixeira para Cozinha 12L Metal Inox Pedal Prata Brinox</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -662,243 +684,57 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>91697550</t>
+          <t>89031495</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+          <t>Ar Condicionado Split Inverter 9000BTUs Frio 220V TCL</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>,90</t>
+          <t>1,779,1,779.90</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>91697550</t>
+          <t>89031495</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+          <t>Ar Condicionado Split Inverter 9000BTUs Frio 220V TCL</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>,90</t>
+          <t>1,779,1,779.90</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>91697550</t>
+          <t>89031495</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
+          <t>Ar Condicionado Split Inverter 9000BTUs Frio 220V TCL</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>,90</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>91697550</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>,90</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>91697550</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>,90</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>91697550</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>,90</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>91697550</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>3,949,90</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>91697550</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>3,949,90</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>91697550</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>3,949,90</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>91697550</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>3.949.90</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>91697550</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>3,949,90</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>91697550</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>3,949,90</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>91697550</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>3,949,90</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>91697550</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Ar condicionado Split 24000 BTUs Quente e Frio 220V Series A1 TCL</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>3,949,90</t>
+          <t>1,779,90</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -908,30 +744,72 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C2"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1">
+        <f>SUBSTITUTE(Planilha1!C2,",",".",1)</f>
+        <v/>
+      </c>
+    </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>55555</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>casa</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>99.99</t>
-        </is>
-      </c>
+      <c r="A2">
+        <f>SUBSTITUTE(Planilha1!C3,",",".",1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <f>SUBSTITUTE(Planilha1!C4,",",".",1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <f>SUBSTITUTE(Planilha1!C5,",",".",1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <f>SUBSTITUTE(Planilha1!C6,",",".",1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <f>SUBSTITUTE(Planilha1!C7,",",".",1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <f>SUBSTITUTE(Planilha1!C8,",",".",1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <f>SUBSTITUTE(Planilha1!C9,",",".",1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <f>SUBSTITUTE(Planilha1!C10,",",".",1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="H12" s="2" t="n"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
amending os 2 códigos
</commit_message>
<xml_diff>
--- a/testes_antes_da_main/teste.xlsx
+++ b/testes_antes_da_main/teste.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
@@ -729,6 +729,57 @@
       <c r="C17" t="inlineStr">
         <is>
           <t>1,779,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>90991005</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 9000BTUs Frio 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1,759,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>89021443</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Depósito para Jardim Manor Resina Cinza 3800 L Keter</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>3,896,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>89021443</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Depósito para Jardim Manor Resina Cinza 3800 L Keter</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>3,896,90</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
testando find prices com csv
</commit_message>
<xml_diff>
--- a/testes_antes_da_main/teste.xlsx
+++ b/testes_antes_da_main/teste.xlsx
@@ -3,11 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Planilha1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -17,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,14 +29,6 @@
       <family val="2"/>
       <b val="1"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,12 +51,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,9 +421,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -783,84 +773,569 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>91949053</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 9000 BTUs Frio Branco 220V Series A2 TCL</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>1,799,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>91949053</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 9000 BTUs Frio Branco 220V Series A2 TCL</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>1,799,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>90376545</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Slipt Inverter 9000BTUs Frio Equation</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>1,799,90</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>9194830491948311</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split Inverter 9000 BTUs Frio Branco 220V Inverter Voice 220V LG</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2,799,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>9194830491948311</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split Inverter 9000 BTUs Frio Branco 220V Inverter Voice 220V LG</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2,799,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>3,999,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>3,999,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>3,999,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>91949060</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 12000 BTUs Frio Branco 220V Series A2 TCL</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2,090,36</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>3,699,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1">
-        <f>SUBSTITUTE(Planilha1!C2,",",".",1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2">
-        <f>SUBSTITUTE(Planilha1!C3,",",".",1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <f>SUBSTITUTE(Planilha1!C4,",",".",1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <f>SUBSTITUTE(Planilha1!C5,",",".",1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <f>SUBSTITUTE(Planilha1!C6,",",".",1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <f>SUBSTITUTE(Planilha1!C7,",",".",1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <f>SUBSTITUTE(Planilha1!C8,",",".",1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <f>SUBSTITUTE(Planilha1!C9,",",".",1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <f>SUBSTITUTE(Planilha1!C10,",",".",1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12">
-      <c r="H12" s="2" t="n"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
extrai valores, mas apenas acima de 10,00 reais
</commit_message>
<xml_diff>
--- a/testes_antes_da_main/teste.xlsx
+++ b/testes_antes_da_main/teste.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
@@ -1334,6 +1334,227 @@
         </is>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>const integers = '3.699'.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>90163990</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Ventilador de Teto com Controle de Parede Fenix 3 Pás 96 cm 127V (110V) Ventisol</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>const integers = '219'.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>90163990</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Ventilador de Teto com Controle de Parede Fenix 3 Pás 96 cm 127V (110V) Ventisol</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>const integers = '219'.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>91989296</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Banheira de Imersão Zen 150x72cm Branco Sensea</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>8.9998.999</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>91989296</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Banheira de Imersão Zen 150x72cm Branco Sensea</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>8.999.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>89062981</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Tapete de Banheiro Antiderrapante Cocoon Poliéster Grafite 40x60cm Sensea</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>99.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>1571352810</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Lâmpada Filamento E14 Ba35 Velachama 2w 127v - Foxlux</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>11.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>9043764190437655</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Cassete Atualle Eco Frio 60000BTUs 220V Elgin</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>13.049.80</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>1571352810</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Lâmpada Filamento E14 Ba35 Velachama 2w 127v - Foxlux</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>11.90</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
organizando o código em funções
</commit_message>
<xml_diff>
--- a/testes_antes_da_main/teste.xlsx
+++ b/testes_antes_da_main/teste.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
@@ -1555,6 +1555,125 @@
         </is>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Series A1 TCL</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
ajustando para nao imprimir os valores None
</commit_message>
<xml_diff>
--- a/testes_antes_da_main/teste.xlsx
+++ b/testes_antes_da_main/teste.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
@@ -1674,6 +1674,125 @@
         </is>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Elite Series A1 Convencional TCL</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>91697550</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 24000 BTUs Quente e Frio Branco 220V Elite Series A1 Convencional TCL</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>3.699.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>86839655</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Cabo Flexível 2,5mm 100m Azul 750V SIL Fios</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>159.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>91989296</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Banheira de Imersão Zen 150x72cm Branco Sensea</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>8.999.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>91989296</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Banheira de Imersão Zen 150x72cm Branco Sensea</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>8.999.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>91989296</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Banheira de Imersão Zen 150x72cm Branco Sensea</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>8.999.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>91989296</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Banheira de Imersão Zen 150x72cm Branco Sensea</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>8.999.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
identando e encontrando mais infos
</commit_message>
<xml_diff>
--- a/testes_antes_da_main/teste.xlsx
+++ b/testes_antes_da_main/teste.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
@@ -1793,6 +1793,91 @@
         </is>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>91989296</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Banheira de Imersão Zen 150x72cm Branco Sensea</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>8.999.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>91989296</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Banheira de Imersão Zen 150x72cm Branco Sensea</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>8.999.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>91989296</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Banheira de Imersão Zen 150x72cm Branco Sensea</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>8.999.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>9092831390928320</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 9000 BTUs Frio Air Volution Springer Midea</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>1.743.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>9092831390928320</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Ar Condicionado Split 9000 BTUs Frio Air Volution Springer Midea</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>1.743.15</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
add checagem se o LM existe no csv
</commit_message>
<xml_diff>
--- a/testes_antes_da_main/teste.xlsx
+++ b/testes_antes_da_main/teste.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
@@ -1878,6 +1878,363 @@
         </is>
       </c>
     </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>91989296</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Banheira de Imersão Zen 150x72cm Branco Sensea</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>8.999.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>86839655</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Cabo Flexível 2,5mm 100m Azul 750V SIL Fios</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>159.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>86839655</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Cabo Flexível 2,5mm 100m Azul 750V SIL Fios</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>159.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>85639624</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Fita Isolante 3M Scotch 33+ Uso Profissional Classe A Preta 19mm x 20m x 0,19mm</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>25.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>89998902</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Gap Roca</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>1.799.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>89998902</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Gap Roca</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>1.799.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>89998902</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Gap Roca</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>1.799.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>89841815</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Lille Sensea</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>804.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>89841815</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Lille Sensea</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>804.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>89841815</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Lille Sensea</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>804.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>89841822</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Lyon Sensea</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>899.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>89841822</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Lyon Sensea</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>899.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>89841822</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Lyon Sensea</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>899.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>89841822</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Lyon Sensea</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>899.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>89841822</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Lyon Sensea</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>899.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>89841822</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Lyon Sensea</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>899.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>89841822</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Lyon Sensea</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>899.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>89841822</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Lyon Sensea</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>899.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>89825036</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Quadra Deca</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>899.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>89825036</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Quadra Deca</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>899.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>89380725</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Porta Papel Higiênico Metal Dupla Sensea</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>62.90</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
atualizando para preparar pro sql
</commit_message>
<xml_diff>
--- a/testes_antes_da_main/teste.xlsx
+++ b/testes_antes_da_main/teste.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C106"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
@@ -2235,6 +2235,40 @@
         </is>
       </c>
     </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>89975816</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Clean Deca</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>1.599.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>90308603</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Torneira Elétrica Bica Alta Branca 220V 5500W Prime Equation</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>83.90</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>